<commit_message>
Mais cartas e mudanças não testadas nos switch's de id de herói pra if's
</commit_message>
<xml_diff>
--- a/WebContent/resource/insert bd cardgame.xlsx
+++ b/WebContent/resource/insert bd cardgame.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="283">
   <si>
     <t>Leanne, a Princesa da Criação</t>
   </si>
@@ -869,6 +869,27 @@
   </si>
   <si>
     <t>(1) Esta carta também pode usar magias de FOGO, ÁGUA, TERRA e VENTO. (2) Se esta carta usar uma magia, durante este turno, seus ataques usarão seu POD em vez da FOR para calcular o dano. (3) Quando esta carta causar dano físico, ela ganha PROT igual ao dano causado.</t>
+  </si>
+  <si>
+    <t>delete from carta where id = 20 or id = 21</t>
+  </si>
+  <si>
+    <t>delete from consumivel where id = 20 or id = 21</t>
+  </si>
+  <si>
+    <t>Explosão de Energia Condensada</t>
+  </si>
+  <si>
+    <t>(1) O usuário causa DANO mágico a um herói inimigo igual ao seu POD.</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Olivia, a Espada Graciosa</t>
+  </si>
+  <si>
+    <t>(1) Quando esta carta usar uma magia, ela ganha   +1 FOR e cura +2 HP.</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="J117" sqref="J117"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="J118" sqref="J118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3799,6 +3820,64 @@
       <c r="H111" t="str">
         <f t="shared" si="2"/>
         <v>INSERT INTO carta values(104,'Reyson, o Filho dos Céus',3,999,4,'(1) Esta carta também pode usar magias de FOGO, ÁGUA, TERRA e VENTO. (2) Se esta carta usar uma magia, durante este turno, seus ataques usarão seu POD em vez da FOR para calcular o dano. (3) Quando esta carta causar dano físico, ela ganha PROT igual ao dano causado.')</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>20</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>50</v>
+      </c>
+      <c r="E115">
+        <v>3</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="H115" t="str">
+        <f t="shared" ref="H115:H116" si="3">CONCATENATE("INSERT INTO carta values(",A115,",'",B115,"',",C115,",",D115,",",E115,",'",F115,"')")</f>
+        <v>INSERT INTO carta values(20,'Explosão de Energia Condensada',0,50,3,'(1) O usuário causa DANO mágico a um herói inimigo igual ao seu POD.')</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>280</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>100</v>
+      </c>
+      <c r="E116">
+        <v>4</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H116" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO carta values(??,'Olivia, a Espada Graciosa',1,100,4,'(1) Quando esta carta usar uma magia, ela ganha   +1 FOR e cura +2 HP.')</v>
       </c>
     </row>
   </sheetData>
@@ -4728,10 +4807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6694,6 +6773,41 @@
       </c>
       <c r="K52">
         <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>280</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>7</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>3</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7070,10 +7184,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7348,7 +7462,7 @@
         <v>3</v>
       </c>
       <c r="F16" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A16,",",B16,",",C16,",",D16,")")</f>
+        <f t="shared" ref="F16:F30" si="1">CONCATENATE("INSERT INTO magia values(",A16,",",B16,",",C16,",",D16,")")</f>
         <v>INSERT INTO magia values(91,4,2,3)</v>
       </c>
     </row>
@@ -7366,7 +7480,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A17,",",B17,",",C17,",",D17,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(92,6,1,1)</v>
       </c>
     </row>
@@ -7384,7 +7498,7 @@
         <v>3</v>
       </c>
       <c r="F18" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A18,",",B18,",",C18,",",D18,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(93,5,2,3)</v>
       </c>
     </row>
@@ -7402,7 +7516,7 @@
         <v>6</v>
       </c>
       <c r="F19" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A19,",",B19,",",C19,",",D19,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(94,2,5,6)</v>
       </c>
     </row>
@@ -7420,7 +7534,7 @@
         <v>3</v>
       </c>
       <c r="F20" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A20,",",B20,",",C20,",",D20,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(95,1,4,3)</v>
       </c>
     </row>
@@ -7438,7 +7552,7 @@
         <v>4</v>
       </c>
       <c r="F21" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A21,",",B21,",",C21,",",D21,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(96,3,3,4)</v>
       </c>
     </row>
@@ -7456,7 +7570,7 @@
         <v>3</v>
       </c>
       <c r="F22" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A22,",",B22,",",C22,",",D22,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(97,3,3,3)</v>
       </c>
     </row>
@@ -7474,7 +7588,7 @@
         <v>3</v>
       </c>
       <c r="F23" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A23,",",B23,",",C23,",",D23,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(98,2,2,3)</v>
       </c>
     </row>
@@ -7492,7 +7606,7 @@
         <v>3</v>
       </c>
       <c r="F24" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A24,",",B24,",",C24,",",D24,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(99,4,2,3)</v>
       </c>
     </row>
@@ -7510,7 +7624,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A25,",",B25,",",C25,",",D25,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(100,5,2,1)</v>
       </c>
     </row>
@@ -7528,7 +7642,7 @@
         <v>3</v>
       </c>
       <c r="F26" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A26,",",B26,",",C26,",",D26,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(101,1,2,3)</v>
       </c>
     </row>
@@ -7546,7 +7660,7 @@
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A27,",",B27,",",C27,",",D27,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(102,5,7,9)</v>
       </c>
     </row>
@@ -7564,8 +7678,26 @@
         <v>5</v>
       </c>
       <c r="F28" t="str">
-        <f>CONCATENATE("INSERT INTO magia values(",A28,",",B28,",",C28,",",D28,")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO magia values(103,6,5,5)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO magia values(20,0,2,1)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mais efeitos adicionados e mudanças em algumas cartas
</commit_message>
<xml_diff>
--- a/WebContent/resource/insert bd cardgame.xlsx
+++ b/WebContent/resource/insert bd cardgame.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliente\git\LES-CardGame\WebContent\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\eclipse-workspace\LES-CardGame\WebContent\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DB2ED8-9035-41AD-85B6-4E44D123B60E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <sheet name="Planilha11" sheetId="11" r:id="rId11"/>
     <sheet name="Planilha12" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="280">
   <si>
     <t>Leanne, a Princesa da Criação</t>
   </si>
@@ -871,19 +872,10 @@
     <t>(1) Esta carta também pode usar magias de FOGO, ÁGUA, TERRA e VENTO. (2) Se esta carta usar uma magia, durante este turno, seus ataques usarão seu POD em vez da FOR para calcular o dano. (3) Quando esta carta causar dano físico, ela ganha PROT igual ao dano causado.</t>
   </si>
   <si>
-    <t>delete from carta where id = 20 or id = 21</t>
-  </si>
-  <si>
-    <t>delete from consumivel where id = 20 or id = 21</t>
-  </si>
-  <si>
     <t>Explosão de Energia Condensada</t>
   </si>
   <si>
     <t>(1) O usuário causa DANO mágico a um herói inimigo igual ao seu POD.</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
   <si>
     <t>Olivia, a Espada Graciosa</t>
@@ -895,7 +887,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1243,11 +1235,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="J118" sqref="J118"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="M114" sqref="M114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3822,22 +3814,12 @@
         <v>INSERT INTO carta values(104,'Reyson, o Filho dos Céus',3,999,4,'(1) Esta carta também pode usar magias de FOGO, ÁGUA, TERRA e VENTO. (2) Se esta carta usar uma magia, durante este turno, seus ataques usarão seu POD em vez da FOR para calcular o dano. (3) Quando esta carta causar dano físico, ela ganha PROT igual ao dano causado.')</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H113" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H114" t="s">
-        <v>277</v>
-      </c>
-    </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>20</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3849,7 +3831,7 @@
         <v>3</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" ref="H115:H116" si="3">CONCATENATE("INSERT INTO carta values(",A115,",'",B115,"',",C115,",",D115,",",E115,",'",F115,"')")</f>
@@ -3857,11 +3839,11 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>280</v>
+      <c r="A116">
+        <v>70</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -3873,11 +3855,11 @@
         <v>4</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO carta values(??,'Olivia, a Espada Graciosa',1,100,4,'(1) Quando esta carta usar uma magia, ela ganha   +1 FOR e cura +2 HP.')</v>
+        <v>INSERT INTO carta values(70,'Olivia, a Espada Graciosa',1,100,4,'(1) Quando esta carta usar uma magia, ela ganha   +1 FOR e cura +2 HP.')</v>
       </c>
     </row>
   </sheetData>
@@ -3887,7 +3869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4537,7 +4519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4588,7 +4570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4806,11 +4788,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="O54" sqref="O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6774,10 +6756,14 @@
       <c r="K52">
         <v>3</v>
       </c>
+      <c r="M52" t="str">
+        <f t="shared" ref="M52:M53" si="1">CONCATENATE("INSERT INTO heroi values(",A52,",",B52,",",C52,",",D52,",",E52,",",F52,",",G52,",",H52,",",I52,",",J52,",",K52,")")</f>
+        <v>INSERT INTO heroi values(104,5,1,12,19,3,7,2,5,6,3)</v>
+      </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>280</v>
+      <c r="A53">
+        <v>70</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -6808,6 +6794,10 @@
       </c>
       <c r="K53">
         <v>2</v>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO heroi values(70,3,5,10,7,3,3,2,3,0,2)</v>
       </c>
     </row>
   </sheetData>
@@ -6816,7 +6806,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -7183,11 +7173,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7706,7 +7696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7740,7 +7730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7778,7 +7768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7918,7 +7908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8601,7 +8591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>